<commit_message>
scheme is working without CASCADEs
</commit_message>
<xml_diff>
--- a/tests/db/testtable/schem.xlsx
+++ b/tests/db/testtable/schem.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3DE741-7950-409F-8485-26335E6A3803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EF23-41F5-4B05-BEA0-2AFBCC718DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>customer</t>
   </si>
@@ -73,9 +73,6 @@
     <t>signerposition</t>
   </si>
   <si>
-    <t>positions</t>
-  </si>
-  <si>
     <t>prim</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>int, autoincr</t>
   </si>
   <si>
-    <t>primary</t>
-  </si>
-  <si>
     <t>spectablescheme</t>
   </si>
   <si>
@@ -151,10 +145,16 @@
     <t>int, def 1</t>
   </si>
   <si>
-    <t>specpattern</t>
-  </si>
-  <si>
-    <t>blob</t>
+    <t>position</t>
+  </si>
+  <si>
+    <t>text, PRIMARY, unique</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>text, primary</t>
   </si>
 </sst>
 </file>
@@ -179,12 +179,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -214,17 +226,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -465,13 +482,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>866775</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -487,9 +504,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3019425" y="962025"/>
-          <a:ext cx="514350" cy="952500"/>
+        <a:xfrm flipH="1">
+          <a:off x="3678555" y="914400"/>
+          <a:ext cx="451485" cy="923925"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -517,10 +534,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -541,8 +558,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4257675" y="952500"/>
-          <a:ext cx="2657475" cy="1905000"/>
+          <a:off x="3497580" y="906780"/>
+          <a:ext cx="3674745" cy="1836420"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -943,7 +960,7 @@
   <dimension ref="B2:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,22 +979,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="E2" s="2" t="s">
-        <v>29</v>
+      <c r="E2" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="6"/>
+      <c r="E3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
@@ -991,19 +1008,16 @@
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="5" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>4</v>
@@ -1014,16 +1028,13 @@
       <c r="J5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="10" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>17</v>
+      <c r="M10" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="5:19" x14ac:dyDescent="0.3">
@@ -1039,27 +1050,27 @@
     </row>
     <row r="12" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="F14" s="2" t="s">
-        <v>19</v>
+      <c r="F14" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="F15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="R15" s="5" t="s">
-        <v>37</v>
+      <c r="F15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="R15" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="5:19" x14ac:dyDescent="0.3">
@@ -1067,15 +1078,15 @@
         <v>6</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="J16" s="4"/>
       <c r="R16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1085,23 +1096,23 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="6"/>
       <c r="R17" s="1">
         <v>1</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
@@ -1109,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
@@ -1117,23 +1128,23 @@
         <v>3</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>23</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>6</v>
@@ -1153,11 +1164,11 @@
       <c r="M22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="N22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
@@ -1189,32 +1200,32 @@
         <v>5</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="H26" s="2" t="s">
-        <v>27</v>
+      <c r="H26" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="H27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" s="6"/>
+      <c r="H27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
       <c r="H28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.3">
@@ -1222,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
almoust all data is added, sql works good
</commit_message>
<xml_diff>
--- a/tests/db/testtable/schem.xlsx
+++ b/tests/db/testtable/schem.xlsx
@@ -3,24 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B07EF23-41F5-4B05-BEA0-2AFBCC718DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248EB473-B0C9-4E94-924B-D4F6D2AE377C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>customer</t>
   </si>
@@ -97,6 +104,9 @@
     <t>int, autoincr</t>
   </si>
   <si>
+    <t>primary</t>
+  </si>
+  <si>
     <t>spectablescheme</t>
   </si>
   <si>
@@ -146,15 +156,6 @@
   </si>
   <si>
     <t>position</t>
-  </si>
-  <si>
-    <t>text, PRIMARY, unique</t>
-  </si>
-  <si>
-    <t>UNIQUE</t>
-  </si>
-  <si>
-    <t>text, primary</t>
   </si>
 </sst>
 </file>
@@ -226,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,9 +240,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -482,13 +480,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -504,9 +502,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3678555" y="914400"/>
-          <a:ext cx="451485" cy="923925"/>
+        <a:xfrm>
+          <a:off x="3019425" y="962025"/>
+          <a:ext cx="514350" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -534,10 +532,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -558,8 +556,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="3497580" y="906780"/>
-          <a:ext cx="3674745" cy="1836420"/>
+          <a:off x="4257675" y="952500"/>
+          <a:ext cx="2657475" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -959,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,22 +977,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="E2" s="5" t="s">
-        <v>27</v>
+      <c r="E2" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="10"/>
+      <c r="E3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
@@ -1011,13 +1009,13 @@
     </row>
     <row r="5" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>4</v>
@@ -1034,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="5:19" x14ac:dyDescent="0.3">
@@ -1050,7 +1048,7 @@
     </row>
     <row r="12" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>17</v>
@@ -1060,17 +1058,17 @@
       </c>
     </row>
     <row r="14" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="5:19" x14ac:dyDescent="0.3">
-      <c r="F15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="10"/>
+      <c r="F15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="9"/>
       <c r="R15" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="5:19" x14ac:dyDescent="0.3">
@@ -1078,13 +1076,13 @@
         <v>6</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J16" s="4"/>
       <c r="R16" s="1" t="s">
@@ -1096,13 +1094,13 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>3</v>
@@ -1112,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
@@ -1120,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.3">
@@ -1128,23 +1126,23 @@
         <v>3</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>6</v>
@@ -1165,10 +1163,10 @@
         <v>11</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
@@ -1200,17 +1198,17 @@
         <v>5</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.3">
       <c r="H26" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
       <c r="H27" s="9" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="I27" s="9"/>
     </row>

</xml_diff>